<commit_message>
modify index input type
</commit_message>
<xml_diff>
--- a/myg-v4/指标信息.xlsx
+++ b/myg-v4/指标信息.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\annmodel\myg-v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0DBF47-9F38-493B-8FD8-2045E97377A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF8FA61-12EA-4E2D-BA7F-852E4E6935C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{E36D9513-DB64-400A-9644-3E5F1B1DCD40}"/>
   </bookViews>
@@ -687,7 +687,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>

</xml_diff>